<commit_message>
Updated spreadsheet roles and locations
</commit_message>
<xml_diff>
--- a/bbf-bioblitz-client/tests/acceptance/steps/BB2017_specs_sheet.xlsx
+++ b/bbf-bioblitz-client/tests/acceptance/steps/BB2017_specs_sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8870" tabRatio="776" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8870" tabRatio="776" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="surveyList" sheetId="11" r:id="rId11"/>
     <sheet name="participantAssignments" sheetId="12" r:id="rId12"/>
     <sheet name="transportList" sheetId="13" r:id="rId13"/>
+    <sheet name="Accom" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="210">
   <si>
     <t>Team</t>
   </si>
@@ -86,9 +87,6 @@
     <t>Drives a transport vehicle</t>
   </si>
   <si>
-    <t>Kitchen Help</t>
-  </si>
-  <si>
     <t>Helps in the kitchen</t>
   </si>
   <si>
@@ -164,9 +162,6 @@
     <t>Bio-security/Hygiene</t>
   </si>
   <si>
-    <t>Manages biosecurity and toilets</t>
-  </si>
-  <si>
     <t>LocationName</t>
   </si>
   <si>
@@ -294,14 +289,400 @@
   </si>
   <si>
     <t>Not Driver</t>
+  </si>
+  <si>
+    <t>AccomRoom</t>
+  </si>
+  <si>
+    <t>Beds</t>
+  </si>
+  <si>
+    <t>Bodies</t>
+  </si>
+  <si>
+    <t>Flat1</t>
+  </si>
+  <si>
+    <t>Flat2</t>
+  </si>
+  <si>
+    <t>Flat3</t>
+  </si>
+  <si>
+    <t>Flat4</t>
+  </si>
+  <si>
+    <t>House_NorfolkLodge_Study</t>
+  </si>
+  <si>
+    <t>House_NorfolkLodge__Bedroom2</t>
+  </si>
+  <si>
+    <t>House_NorfolkLodge__Bedroom3</t>
+  </si>
+  <si>
+    <t>House_NorfolkLodge__Bedroom4</t>
+  </si>
+  <si>
+    <t>House_NorfolkLodge__Bedroom5</t>
+  </si>
+  <si>
+    <t>House_NorfolkLodge__Porch</t>
+  </si>
+  <si>
+    <t>BoyDorm_Room1</t>
+  </si>
+  <si>
+    <t>BoyDorm_Room2</t>
+  </si>
+  <si>
+    <t>BoyDorm_Room3</t>
+  </si>
+  <si>
+    <t>BoyDorm_Room4</t>
+  </si>
+  <si>
+    <t>BoyDorm_Room5</t>
+  </si>
+  <si>
+    <t>BoyDorm_Room6</t>
+  </si>
+  <si>
+    <t>BoyDorm_Room7</t>
+  </si>
+  <si>
+    <t>GirlDorm_Room8</t>
+  </si>
+  <si>
+    <t>GirlDorm_Room9</t>
+  </si>
+  <si>
+    <t>GirlDorm_Room10</t>
+  </si>
+  <si>
+    <t>GirlDorm_Room11</t>
+  </si>
+  <si>
+    <t>GirlDorm_Room12</t>
+  </si>
+  <si>
+    <t>GirlDorm_Room13</t>
+  </si>
+  <si>
+    <t>GirlDorm_Room14</t>
+  </si>
+  <si>
+    <t>GirlDorm_Room15</t>
+  </si>
+  <si>
+    <t>MotorHome_Site1</t>
+  </si>
+  <si>
+    <t>MotorHome_Site2</t>
+  </si>
+  <si>
+    <t>MotorHome_Site3</t>
+  </si>
+  <si>
+    <t>MotorHome_Site4</t>
+  </si>
+  <si>
+    <t>MotorHome_Site5</t>
+  </si>
+  <si>
+    <t>MotorHome_Site6</t>
+  </si>
+  <si>
+    <t>MotorHome_Site7</t>
+  </si>
+  <si>
+    <t>MotorHome_Site8</t>
+  </si>
+  <si>
+    <t>MotorHome_Site9</t>
+  </si>
+  <si>
+    <t>MotorHome_Site10</t>
+  </si>
+  <si>
+    <t>MotorHome_Site11</t>
+  </si>
+  <si>
+    <t>MotorHome_Site12</t>
+  </si>
+  <si>
+    <t>MotorHome_Site13</t>
+  </si>
+  <si>
+    <t>MotorHome_Site14</t>
+  </si>
+  <si>
+    <t>MotorHome_Site15</t>
+  </si>
+  <si>
+    <t>MotorHome_Site16</t>
+  </si>
+  <si>
+    <t>MotorHome_Site17</t>
+  </si>
+  <si>
+    <t>MotorHome_Site18</t>
+  </si>
+  <si>
+    <t>MotorHome_Site19</t>
+  </si>
+  <si>
+    <t>MotorHome_Site20</t>
+  </si>
+  <si>
+    <t>Tent_Site1</t>
+  </si>
+  <si>
+    <t>Tent_Site2</t>
+  </si>
+  <si>
+    <t>Tent_Site3</t>
+  </si>
+  <si>
+    <t>Tent_Site4</t>
+  </si>
+  <si>
+    <t>Tent_Site5</t>
+  </si>
+  <si>
+    <t>Tent_Site6</t>
+  </si>
+  <si>
+    <t>Tent_Site7</t>
+  </si>
+  <si>
+    <t>Tent_Site8</t>
+  </si>
+  <si>
+    <t>Tent_Site9</t>
+  </si>
+  <si>
+    <t>Tent_Site10</t>
+  </si>
+  <si>
+    <t>Tent_Site11</t>
+  </si>
+  <si>
+    <t>Tent_Site12</t>
+  </si>
+  <si>
+    <t>Tent_Site13</t>
+  </si>
+  <si>
+    <t>Tent_Site14</t>
+  </si>
+  <si>
+    <t>Tent_Site15</t>
+  </si>
+  <si>
+    <t>Tent_Site16</t>
+  </si>
+  <si>
+    <t>Tent_Site17</t>
+  </si>
+  <si>
+    <t>Tent_Site18</t>
+  </si>
+  <si>
+    <t>Tent_Site19</t>
+  </si>
+  <si>
+    <t>Tent_Site20</t>
+  </si>
+  <si>
+    <t>Liases with scientists and survey leaders</t>
+  </si>
+  <si>
+    <t>Manages BaseCamp</t>
+  </si>
+  <si>
+    <t>Event Manager</t>
+  </si>
+  <si>
+    <t>Manages BioBlitz event</t>
+  </si>
+  <si>
+    <t>Manages Bio-security/Hygiene</t>
+  </si>
+  <si>
+    <t>Manages evaluation surveys</t>
+  </si>
+  <si>
+    <t>Manages IT</t>
+  </si>
+  <si>
+    <t>Manages SocialMedia</t>
+  </si>
+  <si>
+    <t>Manages BioBlitz data</t>
+  </si>
+  <si>
+    <t>Manages FirstAid team</t>
+  </si>
+  <si>
+    <t>Bio-security/Hygiene Assistant</t>
+  </si>
+  <si>
+    <t>Helps with biosecurity and toilets</t>
+  </si>
+  <si>
+    <t>Kitchen Assistant</t>
+  </si>
+  <si>
+    <t>Manages Coast Field Site</t>
+  </si>
+  <si>
+    <t>Manages Forest Field Site</t>
+  </si>
+  <si>
+    <t>Manages Plains Field Site</t>
+  </si>
+  <si>
+    <t>FieldSite Assistant - Coast</t>
+  </si>
+  <si>
+    <t>FieldSite Assistant - Forest</t>
+  </si>
+  <si>
+    <t>FieldSite Assistant - Plains</t>
+  </si>
+  <si>
+    <t>SocialMedia Assistant</t>
+  </si>
+  <si>
+    <t>Helps with Coast Field Site</t>
+  </si>
+  <si>
+    <t>Helps with Forest Field Site</t>
+  </si>
+  <si>
+    <t>Helps with Plains Field Site</t>
+  </si>
+  <si>
+    <t>Scientist Coordinator</t>
+  </si>
+  <si>
+    <t>FirstAid Coordinator</t>
+  </si>
+  <si>
+    <t>M&amp;E Coordinator</t>
+  </si>
+  <si>
+    <t>B&amp;H Coordinator</t>
+  </si>
+  <si>
+    <t>Kitchen Coordinator</t>
+  </si>
+  <si>
+    <t>SocialMedia Coordinator</t>
+  </si>
+  <si>
+    <t>IT Coordinator</t>
+  </si>
+  <si>
+    <t>Data Coordinator</t>
+  </si>
+  <si>
+    <t>Pre-Event Set-up</t>
+  </si>
+  <si>
+    <t>Prepares and recce's field sites</t>
+  </si>
+  <si>
+    <t>Photography Coordinator</t>
+  </si>
+  <si>
+    <t>Video Coordinator</t>
+  </si>
+  <si>
+    <t>Manages Photography content</t>
+  </si>
+  <si>
+    <t>Manages Video content</t>
+  </si>
+  <si>
+    <t>Helps with SocialMedia, Blogging</t>
+  </si>
+  <si>
+    <t>Equipment Coordinator</t>
+  </si>
+  <si>
+    <t>Transport Coordintor</t>
+  </si>
+  <si>
+    <t>Manages Transport logistics</t>
+  </si>
+  <si>
+    <t>Manages Equipment requirement</t>
+  </si>
+  <si>
+    <t>Manages Kitchen and Meals</t>
+  </si>
+  <si>
+    <t>IT Assistant</t>
+  </si>
+  <si>
+    <t>Helps with IT</t>
+  </si>
+  <si>
+    <t>Data Assistant</t>
+  </si>
+  <si>
+    <t>Helps with Data</t>
+  </si>
+  <si>
+    <t>Helps with managing BaseCamp</t>
+  </si>
+  <si>
+    <t>BaseCamp Site Coordinator</t>
+  </si>
+  <si>
+    <t>Field Site Coordinator - Coast</t>
+  </si>
+  <si>
+    <t>Field Site Coordinator - Forest</t>
+  </si>
+  <si>
+    <t>Field Site Coordinator - Plains</t>
+  </si>
+  <si>
+    <t>BaseCamp Site Assistant</t>
+  </si>
+  <si>
+    <t>BaseCamp Registration Coordinator</t>
+  </si>
+  <si>
+    <t>Manages registrations</t>
+  </si>
+  <si>
+    <t>M&amp;E Assistant</t>
+  </si>
+  <si>
+    <t>Helps with evaluation surveys</t>
+  </si>
+  <si>
+    <t>Tarkine Wilderness Lodge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -329,9 +710,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,7 +1032,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -710,34 +1093,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -763,27 +1146,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
         <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -791,13 +1174,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -805,13 +1188,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -819,13 +1202,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -833,13 +1216,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -867,33 +1250,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>71</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>72</v>
-      </c>
-      <c r="D1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -901,16 +1284,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -918,16 +1301,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -935,16 +1318,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -952,16 +1335,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -969,16 +1352,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -986,16 +1369,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1003,16 +1386,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -1027,7 +1410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1040,54 +1423,54 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -1095,46 +1478,2111 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
         <v>83</v>
-      </c>
-      <c r="C8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C186"/>
+  <sheetViews>
+    <sheetView topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
+    <col min="2" max="3" width="8.81640625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="3">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="3">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="3">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="3">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="3">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="3">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="3">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="3">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="3">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="3">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="3">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="3">
+        <v>23</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="3">
+        <v>24</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="3">
+        <v>25</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="3">
+        <v>26</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="3">
+        <v>27</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="3">
+        <v>28</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="3">
+        <v>29</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="3">
+        <v>30</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="3">
+        <v>31</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="3">
+        <v>32</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="3">
+        <v>33</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="3">
+        <v>34</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="3">
+        <v>35</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="3">
+        <v>36</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="3">
+        <v>37</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="3">
+        <v>38</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="3">
+        <v>39</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="3">
+        <v>40</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="3">
+        <v>41</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="3">
+        <v>42</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="3">
+        <v>43</v>
+      </c>
+      <c r="C44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="3">
+        <v>44</v>
+      </c>
+      <c r="C45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="3">
+        <v>45</v>
+      </c>
+      <c r="C46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="3">
+        <v>46</v>
+      </c>
+      <c r="C47" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" s="3">
+        <v>47</v>
+      </c>
+      <c r="C48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="3">
+        <v>48</v>
+      </c>
+      <c r="C49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="3">
+        <v>49</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="3">
+        <v>50</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="3">
+        <v>51</v>
+      </c>
+      <c r="C52" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="3">
+        <v>52</v>
+      </c>
+      <c r="C53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="3">
+        <v>53</v>
+      </c>
+      <c r="C54" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="3">
+        <v>54</v>
+      </c>
+      <c r="C55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="3">
         <v>55</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C56" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57" s="3">
+        <v>56</v>
+      </c>
+      <c r="C57" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" s="3">
+        <v>57</v>
+      </c>
+      <c r="C58" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="3">
+        <v>58</v>
+      </c>
+      <c r="C59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="3">
+        <v>59</v>
+      </c>
+      <c r="C60" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" s="3">
+        <v>60</v>
+      </c>
+      <c r="C61" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" s="3">
+        <v>61</v>
+      </c>
+      <c r="C62" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B63" s="3">
+        <v>62</v>
+      </c>
+      <c r="C63" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64" s="3">
+        <v>63</v>
+      </c>
+      <c r="C64" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B65" s="3">
+        <v>64</v>
+      </c>
+      <c r="C65" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" s="3">
+        <v>65</v>
+      </c>
+      <c r="C66" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B67" s="3">
+        <v>66</v>
+      </c>
+      <c r="C67" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" s="3">
+        <v>67</v>
+      </c>
+      <c r="C68" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" s="3">
+        <v>68</v>
+      </c>
+      <c r="C69" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" s="3">
+        <v>69</v>
+      </c>
+      <c r="C70" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B71" s="3">
+        <v>70</v>
+      </c>
+      <c r="C71" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B72" s="3">
+        <v>71</v>
+      </c>
+      <c r="C72" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" s="3">
+        <v>72</v>
+      </c>
+      <c r="C73" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74" s="3">
+        <v>73</v>
+      </c>
+      <c r="C74" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B75" s="3">
+        <v>74</v>
+      </c>
+      <c r="C75" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B76" s="3">
+        <v>75</v>
+      </c>
+      <c r="C76" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B77" s="3">
+        <v>76</v>
+      </c>
+      <c r="C77" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78" s="3">
+        <v>77</v>
+      </c>
+      <c r="C78" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B79" s="3">
+        <v>78</v>
+      </c>
+      <c r="C79" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B80" s="3">
+        <v>79</v>
+      </c>
+      <c r="C80" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B81" s="3">
+        <v>80</v>
+      </c>
+      <c r="C81" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B82" s="3">
+        <v>81</v>
+      </c>
+      <c r="C82" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B83" s="3">
+        <v>82</v>
+      </c>
+      <c r="C83" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B84" s="3">
+        <v>83</v>
+      </c>
+      <c r="C84" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B85" s="3">
         <v>84</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C85" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" s="3">
         <v>85</v>
+      </c>
+      <c r="C86" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B87" s="3">
+        <v>86</v>
+      </c>
+      <c r="C87" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B88" s="3">
+        <v>87</v>
+      </c>
+      <c r="C88" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B89" s="3">
+        <v>88</v>
+      </c>
+      <c r="C89" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" s="3">
+        <v>89</v>
+      </c>
+      <c r="C90" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" s="3">
+        <v>90</v>
+      </c>
+      <c r="C91" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92" s="3">
+        <v>91</v>
+      </c>
+      <c r="C92" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B93" s="3">
+        <v>92</v>
+      </c>
+      <c r="C93" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B94" s="3">
+        <v>93</v>
+      </c>
+      <c r="C94" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B95" s="3">
+        <v>94</v>
+      </c>
+      <c r="C95" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B96" s="3">
+        <v>95</v>
+      </c>
+      <c r="C96" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B97" s="3">
+        <v>96</v>
+      </c>
+      <c r="C97" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B98" s="3">
+        <v>97</v>
+      </c>
+      <c r="C98" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B99" s="3">
+        <v>98</v>
+      </c>
+      <c r="C99" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B100" s="3">
+        <v>99</v>
+      </c>
+      <c r="C100" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" s="3">
+        <v>100</v>
+      </c>
+      <c r="C101" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B102" s="3">
+        <v>101</v>
+      </c>
+      <c r="C102" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B103" s="3">
+        <v>102</v>
+      </c>
+      <c r="C103" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" s="3">
+        <v>103</v>
+      </c>
+      <c r="C104" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105" s="3">
+        <v>104</v>
+      </c>
+      <c r="C105" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" s="3">
+        <v>105</v>
+      </c>
+      <c r="C106" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B107" s="3">
+        <v>106</v>
+      </c>
+      <c r="C107" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B108" s="3">
+        <v>107</v>
+      </c>
+      <c r="C108" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B109" s="3">
+        <v>108</v>
+      </c>
+      <c r="C109" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B110" s="3">
+        <v>109</v>
+      </c>
+      <c r="C110" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B111" s="3">
+        <v>110</v>
+      </c>
+      <c r="C111" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B112" s="3">
+        <v>111</v>
+      </c>
+      <c r="C112" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B113" s="3">
+        <v>112</v>
+      </c>
+      <c r="C113" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B114" s="3">
+        <v>113</v>
+      </c>
+      <c r="C114" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B115" s="3">
+        <v>114</v>
+      </c>
+      <c r="C115" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B116" s="3">
+        <v>115</v>
+      </c>
+      <c r="C116" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B117" s="3">
+        <v>116</v>
+      </c>
+      <c r="C117" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B118" s="3">
+        <v>117</v>
+      </c>
+      <c r="C118" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B119" s="3">
+        <v>118</v>
+      </c>
+      <c r="C119" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B120" s="3">
+        <v>119</v>
+      </c>
+      <c r="C120" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B121" s="3">
+        <v>120</v>
+      </c>
+      <c r="C121" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B122" s="3">
+        <v>121</v>
+      </c>
+      <c r="C122" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B123" s="3">
+        <v>122</v>
+      </c>
+      <c r="C123" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B124" s="3">
+        <v>123</v>
+      </c>
+      <c r="C124" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B125" s="3">
+        <v>124</v>
+      </c>
+      <c r="C125" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B126" s="3">
+        <v>125</v>
+      </c>
+      <c r="C126" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B127" s="3">
+        <v>126</v>
+      </c>
+      <c r="C127" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B128" s="3">
+        <v>127</v>
+      </c>
+      <c r="C128" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B129" s="3">
+        <v>128</v>
+      </c>
+      <c r="C129" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B130" s="3">
+        <v>129</v>
+      </c>
+      <c r="C130" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B131" s="3">
+        <v>130</v>
+      </c>
+      <c r="C131" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B132" s="3">
+        <v>131</v>
+      </c>
+      <c r="C132" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B133" s="3">
+        <v>132</v>
+      </c>
+      <c r="C133" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B134" s="3">
+        <v>133</v>
+      </c>
+      <c r="C134" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B135" s="3">
+        <v>134</v>
+      </c>
+      <c r="C135" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B136" s="3">
+        <v>135</v>
+      </c>
+      <c r="C136" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B137" s="3">
+        <v>136</v>
+      </c>
+      <c r="C137" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B138" s="3">
+        <v>137</v>
+      </c>
+      <c r="C138" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B139" s="3">
+        <v>138</v>
+      </c>
+      <c r="C139" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B140" s="3">
+        <v>139</v>
+      </c>
+      <c r="C140" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B141" s="3">
+        <v>140</v>
+      </c>
+      <c r="C141" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B142" s="3">
+        <v>141</v>
+      </c>
+      <c r="C142" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B143" s="3">
+        <v>142</v>
+      </c>
+      <c r="C143" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B144" s="3">
+        <v>143</v>
+      </c>
+      <c r="C144" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B145" s="3">
+        <v>144</v>
+      </c>
+      <c r="C145" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B146" s="3">
+        <v>145</v>
+      </c>
+      <c r="C146" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B147" s="3">
+        <v>146</v>
+      </c>
+      <c r="C147" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B148" s="3">
+        <v>147</v>
+      </c>
+      <c r="C148" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B149" s="3">
+        <v>148</v>
+      </c>
+      <c r="C149" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B150" s="3">
+        <v>149</v>
+      </c>
+      <c r="C150" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B151" s="3">
+        <v>150</v>
+      </c>
+      <c r="C151" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B152" s="3">
+        <v>151</v>
+      </c>
+      <c r="C152" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B153" s="3">
+        <v>152</v>
+      </c>
+      <c r="C153" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B154" s="3">
+        <v>153</v>
+      </c>
+      <c r="C154" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B155" s="3">
+        <v>154</v>
+      </c>
+      <c r="C155" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B156" s="3">
+        <v>155</v>
+      </c>
+      <c r="C156" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A157" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B157" s="3">
+        <v>156</v>
+      </c>
+      <c r="C157" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A158" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B158" s="3">
+        <v>157</v>
+      </c>
+      <c r="C158" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A159" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B159" s="3">
+        <v>158</v>
+      </c>
+      <c r="C159" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A160" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B160" s="3">
+        <v>159</v>
+      </c>
+      <c r="C160" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B161" s="3">
+        <v>160</v>
+      </c>
+      <c r="C161" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A162" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B162" s="3">
+        <v>161</v>
+      </c>
+      <c r="C162" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A163" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B163" s="3">
+        <v>162</v>
+      </c>
+      <c r="C163" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B164" s="3">
+        <v>163</v>
+      </c>
+      <c r="C164" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A165" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B165" s="3">
+        <v>164</v>
+      </c>
+      <c r="C165" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A166" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B166" s="3">
+        <v>165</v>
+      </c>
+      <c r="C166" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A167" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B167" s="3">
+        <v>166</v>
+      </c>
+      <c r="C167" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B168" s="3">
+        <v>167</v>
+      </c>
+      <c r="C168" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B169" s="3">
+        <v>168</v>
+      </c>
+      <c r="C169" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B170" s="3">
+        <v>169</v>
+      </c>
+      <c r="C170" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B171" s="3">
+        <v>170</v>
+      </c>
+      <c r="C171" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B172" s="3">
+        <v>171</v>
+      </c>
+      <c r="C172" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A173" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B173" s="3">
+        <v>172</v>
+      </c>
+      <c r="C173" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A174" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B174" s="3">
+        <v>173</v>
+      </c>
+      <c r="C174" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A175" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B175" s="3">
+        <v>174</v>
+      </c>
+      <c r="C175" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B176" s="3">
+        <v>175</v>
+      </c>
+      <c r="C176" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A177" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B177" s="3">
+        <v>176</v>
+      </c>
+      <c r="C177" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A178" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B178" s="3">
+        <v>177</v>
+      </c>
+      <c r="C178" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A179" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B179" s="3">
+        <v>178</v>
+      </c>
+      <c r="C179" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A180" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B180" s="3">
+        <v>179</v>
+      </c>
+      <c r="C180" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A181" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B181" s="3">
+        <v>180</v>
+      </c>
+      <c r="C181" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A182" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B182" s="3">
+        <v>181</v>
+      </c>
+      <c r="C182" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A183" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B183" s="3">
+        <v>182</v>
+      </c>
+      <c r="C183" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A184" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B184" s="3">
+        <v>183</v>
+      </c>
+      <c r="C184" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A185" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B185" s="3">
+        <v>184</v>
+      </c>
+      <c r="C185" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A186" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B186" s="3">
+        <v>185</v>
+      </c>
+      <c r="C186" s="3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1144,72 +3592,391 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" customWidth="1"/>
-    <col min="2" max="2" width="28.7265625" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" customWidth="1"/>
+    <col min="2" max="2" width="34.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B25" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>204</v>
+      </c>
+      <c r="B27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" t="s">
+        <v>198</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" t="s">
+        <v>208</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1232,7 +3999,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1240,10 +4007,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1268,18 +4035,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1">
         <v>43063.875</v>
@@ -1290,7 +4057,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1">
         <v>43064.208333333336</v>
@@ -1301,7 +4068,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1">
         <v>43064.375</v>
@@ -1312,7 +4079,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
         <v>43064.541666666664</v>
@@ -1323,7 +4090,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1">
         <v>43064.875</v>
@@ -1334,7 +4101,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1">
         <v>43065.208333333336</v>
@@ -1345,7 +4112,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1">
         <v>43065.375</v>
@@ -1356,7 +4123,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1">
         <v>43065.541666666664</v>
@@ -1387,16 +4154,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1404,13 +4171,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1420,21 +4187,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" customWidth="1"/>
+    <col min="1" max="1" width="24.36328125" customWidth="1"/>
     <col min="2" max="2" width="32.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1442,26 +4209,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -1486,27 +4261,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>16</v>
@@ -1534,16 +4309,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -1551,19 +4326,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1587,15 +4362,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1603,7 +4378,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -1611,7 +4386,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>8</v>

</xml_diff>

<commit_message>
Update to 1 Sep; test data
updates specs sheet and uploading CSV data file for testing
</commit_message>
<xml_diff>
--- a/bbf-bioblitz-client/tests/acceptance/steps/BB2017_specs_sheet.xlsx
+++ b/bbf-bioblitz-client/tests/acceptance/steps/BB2017_specs_sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8870" tabRatio="776" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8870" tabRatio="776" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1037,7 +1037,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
+    <col min="2" max="2" width="40.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -3594,7 +3595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
@@ -4189,7 +4190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -4297,7 +4298,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>